<commit_message>
Minor re-organization to move watchdog and httpendpoints to lib folder
</commit_message>
<xml_diff>
--- a/requirements/pyGooIbClient Requirements.xlsx
+++ b/requirements/pyGooIbClient Requirements.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Feature</t>
   </si>
@@ -34,12 +34,6 @@
     <t>Provide a POST interface</t>
   </si>
   <si>
-    <t>Automatically re-authenticate client sessions at a configurable interval</t>
-  </si>
-  <si>
-    <t>Automatically re-authenticate websessions at a configurable interval</t>
-  </si>
-  <si>
     <t>Method to Request streaming market data from IB Client</t>
   </si>
   <si>
@@ -49,9 +43,6 @@
     <t>Username and account password stored in enviromental variables, not in system code</t>
   </si>
   <si>
-    <t>Commands and operations will build on basic library using separate classes/files</t>
-  </si>
-  <si>
     <t>System can recover and retrieve state from host reboot</t>
   </si>
   <si>
@@ -61,15 +52,6 @@
     <t>System can recover and retrieve state from loss of communication with Client Portal</t>
   </si>
   <si>
-    <t>CLI parameter to tell which interface(s) used for external applications (ROS2, zeroMQ, etc.)</t>
-  </si>
-  <si>
-    <t>CLI parameter to configure "tickle" period for client and websessions</t>
-  </si>
-  <si>
-    <t>CLI use python argparse library</t>
-  </si>
-  <si>
     <t>CLI flags use standard Linux format</t>
   </si>
   <si>
@@ -115,7 +97,31 @@
     <t>provide a ROS2 interface</t>
   </si>
   <si>
-    <t>provide a zeroMQ interface</t>
+    <t>Logging</t>
+  </si>
+  <si>
+    <t>Log files will cover a single day</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>All configurable parameters will be stored in YAML format</t>
+  </si>
+  <si>
+    <t>Configuration files will be stored in the folder where used [default] but may use an alternate path if provided</t>
+  </si>
+  <si>
+    <t>Interfaces</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>User Interface</t>
+  </si>
+  <si>
+    <t>Provide a configurable time between IB Client "Tickle" events</t>
   </si>
 </sst>
 </file>
@@ -168,8 +174,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C75" totalsRowShown="0">
-  <autoFilter ref="A1:C75"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C72" totalsRowShown="0">
+  <autoFilter ref="A1:C72"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Feature"/>
     <tableColumn id="2" name="Category"/>
@@ -466,16 +472,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="136.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -491,11 +497,17 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -511,138 +523,153 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
       <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working commit for configuration. Also some minor file reorg in lib folder
</commit_message>
<xml_diff>
--- a/requirements/pyGooIbClient Requirements.xlsx
+++ b/requirements/pyGooIbClient Requirements.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Feature</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Method to Request account information from IB Client</t>
   </si>
   <si>
-    <t>Username and account password stored in enviromental variables, not in system code</t>
-  </si>
-  <si>
     <t>System can recover and retrieve state from host reboot</t>
   </si>
   <si>
@@ -106,12 +103,6 @@
     <t>Configuration</t>
   </si>
   <si>
-    <t>All configurable parameters will be stored in YAML format</t>
-  </si>
-  <si>
-    <t>Configuration files will be stored in the folder where used [default] but may use an alternate path if provided</t>
-  </si>
-  <si>
     <t>Interfaces</t>
   </si>
   <si>
@@ -122,6 +113,21 @@
   </si>
   <si>
     <t>Provide a configurable time between IB Client "Tickle" events</t>
+  </si>
+  <si>
+    <t>A configured parameter may be optional or required</t>
+  </si>
+  <si>
+    <t>Configuration parameters stored using ConfigObj format</t>
+  </si>
+  <si>
+    <t>Configuration specification shall be supported</t>
+  </si>
+  <si>
+    <t>configuration path shall default to root directory but optional path shall be supported</t>
+  </si>
+  <si>
+    <t>parameter access shall be via a string path rather than multiple dictionaries</t>
   </si>
 </sst>
 </file>
@@ -174,8 +180,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C72" totalsRowShown="0">
-  <autoFilter ref="A1:C72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C76" totalsRowShown="0">
+  <autoFilter ref="A1:C76"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Feature"/>
     <tableColumn id="2" name="Category"/>
@@ -472,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +504,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -506,7 +512,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -523,11 +529,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -537,12 +540,12 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -552,124 +555,143 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
         <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
       <c r="C17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
         <v>33</v>
       </c>
-      <c r="C22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a bunch of unit tests for configuration
</commit_message>
<xml_diff>
--- a/requirements/pyGooIbClient Requirements.xlsx
+++ b/requirements/pyGooIbClient Requirements.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Feature</t>
   </si>
@@ -121,13 +121,16 @@
     <t>Configuration parameters stored using ConfigObj format</t>
   </si>
   <si>
-    <t>Configuration specification shall be supported</t>
-  </si>
-  <si>
-    <t>configuration path shall default to root directory but optional path shall be supported</t>
-  </si>
-  <si>
     <t>parameter access shall be via a string path rather than multiple dictionaries</t>
+  </si>
+  <si>
+    <t>Configuration specification shall be required</t>
+  </si>
+  <si>
+    <t>providing no file names will default to 'config.ini' and 'config_spec.ini', for the configuration and specification files, respectively</t>
+  </si>
+  <si>
+    <t>if configuration files are not found in the local directory, each higher directory shall be searched for the files until a specific folder is reached</t>
   </si>
 </sst>
 </file>
@@ -180,8 +183,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C76" totalsRowShown="0">
-  <autoFilter ref="A1:C76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C77" totalsRowShown="0">
+  <autoFilter ref="A1:C77"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Feature"/>
     <tableColumn id="2" name="Category"/>
@@ -478,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +598,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>29</v>
       </c>
@@ -603,7 +606,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
@@ -611,86 +617,103 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>11</v>
+      </c>
       <c r="B20" t="s">
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11</v>
+      </c>
       <c r="B23" t="s">
         <v>28</v>
       </c>
       <c r="C23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>31</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>